<commit_message>
change lecturer _ form
</commit_message>
<xml_diff>
--- a/PMS/forms/lecturer_form.xlsx
+++ b/PMS/forms/lecturer_form.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TRƯỜNG ĐH QUỐC TẾ MIỀN ĐÔNG</t>
   </si>
@@ -63,13 +63,47 @@
     <t>Họ và tên Giảng viên chấm điểm:</t>
   </si>
   <si>
-    <t>Nhận xét</t>
-  </si>
-  <si>
-    <t>Góp ý</t>
-  </si>
-  <si>
     <t>Giảng viên</t>
+  </si>
+  <si>
+    <t>Nội dung chấm điểm</t>
+  </si>
+  <si>
+    <t>Điểm tối đa</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>PHẦN BÁO CÁO</t>
+  </si>
+  <si>
+    <t>Nội dung đề tai đạt yêu cầu đặt ra, 
+có tính khoa học</t>
+  </si>
+  <si>
+    <t>Phương pháp thực hiện tốt</t>
+  </si>
+  <si>
+    <t>Kết quả đề tài có áp dụng thực tế</t>
+  </si>
+  <si>
+    <t>Đề tài mới hoặc phương pháp thực
+ hiện có tính sáng tạo</t>
+  </si>
+  <si>
+    <t>PHẦN TRẢ LỜI</t>
+  </si>
+  <si>
+    <t>TỔNG CỘNG</t>
+  </si>
+  <si>
+    <t>Trình bày tốt (Chuẩn bị slide tốt, 
+trình bày rõ ràng đúng thời hạn)</t>
+  </si>
+  <si>
+    <t>Trả lời tập trung vào đề tài,
+trả lời tốt câu hỏi</t>
   </si>
 </sst>
 </file>
@@ -116,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,110 +173,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -253,37 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -298,11 +203,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,10 +492,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,53 +506,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -670,26 +575,26 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -767,59 +672,115 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="E21" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="13">
+        <v>80</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="8">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="8">
+        <v>20</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="8">
+        <v>20</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="8">
         <v>10</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="24"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="24"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="24"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="24"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="24"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="8">
+        <v>10</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="23"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="7" t="s">
-        <v>12</v>
+      <c r="B28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="13">
+        <v>20</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="8">
+        <v>20</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="13">
+        <v>100</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:D26"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="C8:F10"/>

</xml_diff>